<commit_message>
penambahan title prediction untuk PRADIO2, perbaikan keluaran output di prediction, perubahan besar kotak base output file name
</commit_message>
<xml_diff>
--- a/build/web/Groutability(Train).xlsx
+++ b/build/web/Groutability(Train).xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\00 Swarm Optimization\NiMOPSJava\web\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25170" windowHeight="10575"/>
   </bookViews>
@@ -16,35 +21,35 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>D10(um)</t>
+    <t>X1</t>
   </si>
   <si>
-    <t>D15(um)</t>
+    <t>X2</t>
   </si>
   <si>
-    <t>Cu</t>
+    <t>X3</t>
   </si>
   <si>
-    <t>Cz</t>
+    <t>X4</t>
   </si>
   <si>
-    <t>e</t>
+    <t>X5</t>
   </si>
   <si>
-    <t>FC</t>
+    <t>X6</t>
   </si>
   <si>
-    <t>W/C</t>
+    <t>X7</t>
   </si>
   <si>
-    <t>Groutability</t>
+    <t>X8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,7 +91,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -102,7 +107,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -144,7 +149,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,9 +181,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,6 +216,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,21 +392,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,7 +433,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>37</v>
       </c>
@@ -452,7 +459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>30</v>
       </c>
@@ -478,7 +485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
@@ -504,7 +511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3.3000000000000003</v>
       </c>
@@ -530,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>18</v>
       </c>
@@ -556,7 +563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>54</v>
       </c>
@@ -582,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>72</v>
       </c>
@@ -608,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>13</v>
       </c>
@@ -634,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>19</v>
       </c>
@@ -660,7 +667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>22</v>
       </c>
@@ -686,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>40</v>
       </c>
@@ -712,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -738,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.8</v>
       </c>
@@ -764,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>28</v>
       </c>
@@ -790,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.8</v>
       </c>
@@ -816,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>47.999999999999993</v>
       </c>
@@ -842,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>21</v>
       </c>
@@ -868,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.6</v>
       </c>
@@ -894,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6.2</v>
       </c>
@@ -920,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -946,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11</v>
       </c>
@@ -972,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>11</v>
       </c>
@@ -998,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1024,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2.5</v>
       </c>
@@ -1050,7 +1057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6.5</v>
       </c>
@@ -1076,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>34</v>
       </c>
@@ -1102,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>12</v>
       </c>
@@ -1128,7 +1135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>23</v>
       </c>
@@ -1154,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>19</v>
       </c>
@@ -1180,7 +1187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.28000000000000003</v>
       </c>
@@ -1206,7 +1213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>80</v>
       </c>
@@ -1232,7 +1239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3.1999999999999997</v>
       </c>
@@ -1258,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>11</v>
       </c>
@@ -1284,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7.2</v>
       </c>
@@ -1310,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>11</v>
       </c>
@@ -1336,7 +1343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1362,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2.2000000000000002</v>
       </c>
@@ -1388,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>13</v>
       </c>
@@ -1414,7 +1421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>74</v>
       </c>
@@ -1440,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>11</v>
       </c>
@@ -1466,7 +1473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>25</v>
       </c>
@@ -1492,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>15</v>
       </c>
@@ -1518,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>19</v>
       </c>
@@ -1544,7 +1551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>26</v>
       </c>
@@ -1570,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3.4000000000000004</v>
       </c>
@@ -1596,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1.2</v>
       </c>
@@ -1622,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1.2</v>
       </c>
@@ -1648,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>75</v>
       </c>
@@ -1674,7 +1681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.30000000000000004</v>
       </c>
@@ -1700,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>74</v>
       </c>
@@ -1726,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>9</v>
       </c>
@@ -1752,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>11</v>
       </c>
@@ -1778,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>15</v>
       </c>
@@ -1804,7 +1811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>21</v>
       </c>
@@ -1830,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>61.000000000000007</v>
       </c>
@@ -1856,7 +1863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>13</v>
       </c>
@@ -1882,7 +1889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>38</v>
       </c>
@@ -1908,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1934,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>30</v>
       </c>
@@ -1960,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3.0000000000000004</v>
       </c>
@@ -1986,7 +1993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>51</v>
       </c>
@@ -2012,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>17</v>
       </c>
@@ -2038,7 +2045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9</v>
       </c>
@@ -2064,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>16</v>
       </c>
@@ -2090,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5.7999999999999989</v>
       </c>
@@ -2116,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>8</v>
       </c>
@@ -2142,7 +2149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>70</v>
       </c>
@@ -2168,7 +2175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0.28000000000000003</v>
       </c>
@@ -2194,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>30</v>
       </c>
@@ -2220,7 +2227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>21</v>
       </c>
@@ -2246,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>22</v>
       </c>
@@ -2272,7 +2279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>13</v>
       </c>
@@ -2298,7 +2305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0.11</v>
       </c>
@@ -2324,7 +2331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>61.000000000000007</v>
       </c>
@@ -2350,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>22</v>
       </c>
@@ -2376,7 +2383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1.9999999999999998</v>
       </c>
@@ -2402,7 +2409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2.1</v>
       </c>
@@ -2428,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>64</v>
       </c>
@@ -2454,7 +2461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2.2000000000000002</v>
       </c>
@@ -2480,7 +2487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>50</v>
       </c>
@@ -2506,7 +2513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>19</v>
       </c>
@@ -2532,7 +2539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>6.0999999999999988</v>
       </c>
@@ -2558,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2584,7 +2591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>8</v>
       </c>
@@ -2610,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>76</v>
       </c>
@@ -2636,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>8</v>
       </c>
@@ -2662,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>52</v>
       </c>
@@ -2688,7 +2695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>38</v>
       </c>
@@ -2714,7 +2721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>5.9999999999999991</v>
       </c>
@@ -2740,7 +2747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>11</v>
       </c>
@@ -2766,7 +2773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>11</v>
       </c>
@@ -2792,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>7.2</v>
       </c>
@@ -2818,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>16</v>
       </c>
@@ -2844,7 +2851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>18</v>
       </c>
@@ -2870,7 +2877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>18</v>
       </c>
@@ -2896,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>47.999999999999993</v>
       </c>
@@ -2922,7 +2929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>24</v>
       </c>
@@ -2948,7 +2955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2.8</v>
       </c>
@@ -2974,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1.7999999999999998</v>
       </c>
@@ -3000,7 +3007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>11</v>
       </c>
@@ -3026,7 +3033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1.08</v>
       </c>
@@ -3052,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>30</v>
       </c>
@@ -3078,7 +3085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>47.999999999999993</v>
       </c>
@@ -3104,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>13</v>
       </c>
@@ -3130,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>51</v>
       </c>
@@ -3156,7 +3163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>16</v>
       </c>
@@ -3182,7 +3189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>14</v>
       </c>
@@ -3208,7 +3215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0.2</v>
       </c>
@@ -3234,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>58</v>
       </c>
@@ -3260,7 +3267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>7</v>
       </c>
@@ -3286,7 +3293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>30</v>
       </c>
@@ -3312,7 +3319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>73</v>
       </c>
@@ -3338,7 +3345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>37</v>
       </c>
@@ -3364,7 +3371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>10</v>
       </c>
@@ -3390,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>10</v>
       </c>
@@ -3416,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>17</v>
       </c>
@@ -3442,7 +3449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>13</v>
       </c>
@@ -3468,7 +3475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1.5999999999999999</v>
       </c>
@@ -3494,7 +3501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>10</v>
       </c>
@@ -3520,7 +3527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>51</v>
       </c>
@@ -3546,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>19</v>
       </c>
@@ -3572,7 +3579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>17</v>
       </c>
@@ -3598,7 +3605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1.5000000000000002</v>
       </c>
@@ -3624,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>24</v>
       </c>
@@ -3650,7 +3657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>29</v>
       </c>
@@ -3676,7 +3683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>3.0000000000000004</v>
       </c>
@@ -3702,7 +3709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>11</v>
       </c>
@@ -3728,7 +3735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>0.1</v>
       </c>
@@ -3754,7 +3761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>21</v>
       </c>
@@ -3780,7 +3787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>17</v>
       </c>
@@ -3806,7 +3813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>25</v>
       </c>
@@ -3832,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>11</v>
       </c>
@@ -3858,7 +3865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>15</v>
       </c>
@@ -3884,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>1.9999999999999998</v>
       </c>
@@ -3910,7 +3917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>0.9</v>
       </c>
@@ -3936,7 +3943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>0.5</v>
       </c>
@@ -3962,7 +3969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>0.83</v>
       </c>
@@ -3988,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>12</v>
       </c>
@@ -4014,7 +4021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>11</v>
       </c>
@@ -4040,7 +4047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>0.6</v>
       </c>
@@ -4066,7 +4073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>13</v>
       </c>
@@ -4092,7 +4099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>72</v>
       </c>
@@ -4118,7 +4125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>85</v>
       </c>
@@ -4144,7 +4151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2.4</v>
       </c>
@@ -4170,7 +4177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>21</v>
       </c>
@@ -4196,7 +4203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>4.8</v>
       </c>
@@ -4222,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>1.1000000000000001</v>
       </c>
@@ -4248,7 +4255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>0.27</v>
       </c>
@@ -4274,7 +4281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>1.2</v>
       </c>
@@ -4300,7 +4307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>73</v>
       </c>
@@ -4326,7 +4333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>1</v>
       </c>
@@ -4352,7 +4359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>9.5</v>
       </c>
@@ -4378,7 +4385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>30</v>
       </c>
@@ -4404,7 +4411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>13</v>
       </c>
@@ -4430,7 +4437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>47.999999999999993</v>
       </c>
@@ -4456,7 +4463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>71</v>
       </c>
@@ -4482,7 +4489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2.5</v>
       </c>
@@ -4508,7 +4515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>10.5</v>
       </c>
@@ -4534,7 +4541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>13</v>
       </c>
@@ -4560,7 +4567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>12</v>
       </c>
@@ -4586,7 +4593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>1</v>
       </c>
@@ -4612,7 +4619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>7</v>
       </c>
@@ -4638,7 +4645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>31</v>
       </c>
@@ -4664,7 +4671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>26</v>
       </c>
@@ -4690,7 +4697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>8</v>
       </c>
@@ -4716,7 +4723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>21</v>
       </c>
@@ -4742,7 +4749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>25</v>
       </c>
@@ -4768,7 +4775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>4.3</v>
       </c>
@@ -4794,7 +4801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>23</v>
       </c>
@@ -4820,7 +4827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>0.94999999999999984</v>
       </c>
@@ -4846,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>0.6</v>
       </c>
@@ -4872,7 +4879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>32</v>
       </c>
@@ -4898,7 +4905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>0.5</v>
       </c>
@@ -4924,7 +4931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>12</v>
       </c>
@@ -4950,7 +4957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>15</v>
       </c>
@@ -4976,7 +4983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>11</v>
       </c>
@@ -5002,7 +5009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>11</v>
       </c>
@@ -5028,7 +5035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>13</v>
       </c>
@@ -5054,7 +5061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>7</v>
       </c>
@@ -5080,7 +5087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>28</v>
       </c>
@@ -5106,7 +5113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>10</v>
       </c>
@@ -5132,7 +5139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>6.2999999999999989</v>
       </c>
@@ -5158,7 +5165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>19</v>
       </c>
@@ -5184,7 +5191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>15</v>
       </c>
@@ -5210,7 +5217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>18</v>
       </c>
@@ -5236,7 +5243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>8.5</v>
       </c>
@@ -5262,7 +5269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>11</v>
       </c>
@@ -5288,7 +5295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>42</v>
       </c>
@@ -5314,7 +5321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>0.9</v>
       </c>
@@ -5340,7 +5347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>11</v>
       </c>
@@ -5366,7 +5373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>4.2</v>
       </c>
@@ -5392,7 +5399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>7</v>
       </c>

</xml_diff>